<commit_message>
Fixed BOM issue with LEDS.
</commit_message>
<xml_diff>
--- a/CAM_OUTPUTS/BOM/I2C_Jog_Controller_CAM_OUTPUT_A4.xlsx
+++ b/CAM_OUTPUTS/BOM/I2C_Jog_Controller_CAM_OUTPUT_A4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="17115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22110" windowHeight="14805"/>
   </bookViews>
   <sheets>
     <sheet name="I2C_Jog_Controller_CAM_OUTPUT_A" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
     <t>Intelligent Control LED Integrated Light Source, 3.5 to 5.3 V, -25 to 80 degC, 4-Pin SMD, RoHS, Tape and Reel</t>
   </si>
   <si>
-    <t>CYC_U7, FHL_U7, HLT_U7, HME_U7, SPN_U7, U1, U5</t>
+    <t>CYC_U7, FHL_U7, HLT_U7, HME_U7, SPN_U7, U1, U2, U3, U4, U5</t>
   </si>
   <si>
     <t>ADA-RGB-1655_V</t>
@@ -748,7 +748,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit missing Q2 from BOM and PNP.
</commit_message>
<xml_diff>
--- a/CAM_OUTPUTS/BOM/I2C_Jog_Controller_CAM_OUTPUT_A4.xlsx
+++ b/CAM_OUTPUTS/BOM/I2C_Jog_Controller_CAM_OUTPUT_A4.xlsx
@@ -194,7 +194,7 @@
     <t>三极管</t>
   </si>
   <si>
-    <t>Q1</t>
+    <t>Q1, Q2</t>
   </si>
   <si>
     <t>SOT-23(SOT-23-3)</t>
@@ -848,7 +848,7 @@
         <v>57</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>